<commit_message>
Deploying to gh-pages from  @ 22e5c61acc108c409124660f25e6740acca7dda4 🚀
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +406,10 @@
         <v>actors</v>
       </c>
       <c r="I1" t="str">
-        <v>aux.reversible</v>
+        <v>output</v>
+      </c>
+      <c r="J1" t="str">
+        <v>reversible</v>
       </c>
     </row>
     <row r="2">
@@ -422,6 +425,9 @@
       <c r="E2" t="str">
         <v>1</v>
       </c>
+      <c r="I2" t="str">
+        <v>true</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -439,6 +445,9 @@
       <c r="G3" t="str">
         <v>comp1</v>
       </c>
+      <c r="I3" t="str">
+        <v>true</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -456,6 +465,9 @@
       <c r="G4" t="str">
         <v>comp1</v>
       </c>
+      <c r="I4" t="str">
+        <v>true</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -474,6 +486,9 @@
         <v>A = 2*B</v>
       </c>
       <c r="I5" t="str">
+        <v>true</v>
+      </c>
+      <c r="J5" t="str">
         <v>false</v>
       </c>
     </row>
@@ -493,7 +508,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>